<commit_message>
ref 3 Table 1
</commit_message>
<xml_diff>
--- a/database/expdata/Ref_03_Table_1.xlsx
+++ b/database/expdata/Ref_03_Table_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/PSU_PHYS496/database/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6408251-38B3-0444-8912-778A84FB6EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB19F86-35B4-A14E-AAF1-BFDB093FBA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1860" windowWidth="20140" windowHeight="12120" xr2:uid="{DB1F62B9-94EC-407E-9271-D1447D94E2A8}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="17">
   <si>
     <t>Q2 (GeV2)</t>
   </si>
@@ -52,69 +52,6 @@
     <t>W (GeV)</t>
   </si>
   <si>
-    <t>7.1</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>0.69</t>
-  </si>
-  <si>
-    <t>0.14</t>
-  </si>
-  <si>
-    <t>3.4</t>
-  </si>
-  <si>
-    <t>0.30</t>
-  </si>
-  <si>
-    <t>2.9</t>
-  </si>
-  <si>
-    <t>0.61</t>
-  </si>
-  <si>
-    <t>0.29</t>
-  </si>
-  <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>1.9</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>0.38</t>
-  </si>
-  <si>
-    <t>0.17</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>0.60</t>
-  </si>
-  <si>
-    <t>0.90</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
     <t>t (GeV2)</t>
   </si>
   <si>
@@ -127,9 +64,6 @@
     <t>obs</t>
   </si>
   <si>
-    <t>dsigma/dt (nb/GeV2)</t>
-  </si>
-  <si>
     <t>stat_u</t>
   </si>
   <si>
@@ -148,20 +82,35 @@
     <t>beam</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>energy</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>nb/GeV2</t>
+  </si>
+  <si>
+    <t>dsigma/dt</t>
+  </si>
+  <si>
+    <t>e+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,9 +136,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -506,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4385159E-F628-4354-B6F3-127FE67EC495}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -518,12 +470,12 @@
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="8" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -532,31 +484,34 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -572,23 +527,26 @@
       <c r="E2" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
+      <c r="F2" s="2">
+        <v>7.1</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.3</v>
       </c>
@@ -598,29 +556,32 @@
       <c r="C3">
         <v>71</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
+      <c r="D3" s="2">
+        <v>8</v>
       </c>
       <c r="E3" s="1">
         <v>1.4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
+      <c r="F3" s="2">
+        <v>1.4</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -633,26 +594,29 @@
       <c r="D4" s="1">
         <v>2.13</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
+      <c r="E4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.69</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.8</v>
       </c>
@@ -668,23 +632,26 @@
       <c r="E5" s="1">
         <v>0.12</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
+      <c r="F5" s="2">
+        <v>0.14000000000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.1</v>
       </c>
@@ -697,26 +664,29 @@
       <c r="D6" s="1">
         <v>13.3</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>6</v>
+      <c r="E6" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3.4</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.3</v>
       </c>
@@ -729,26 +699,29 @@
       <c r="D7" s="1">
         <v>3.99</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
+      <c r="E7" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.69</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -758,29 +731,32 @@
       <c r="C8">
         <v>82</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -793,154 +769,30 @@
       <c r="D9" s="1">
         <v>0.36</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>5</v>
+      <c r="E9" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.14000000000000001</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>0.1</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>82</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0.3</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>82</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3.44</v>
-      </c>
-      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>0.5</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>82</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>0.8</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>82</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>